<commit_message>
I hope the divergence is fixed
</commit_message>
<xml_diff>
--- a/TestingIterative.xlsx
+++ b/TestingIterative.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\source\repos\ostephagus\NEAProjectCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FF60A7E5-54AC-4D6C-9DF0-CD006EEFFFAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99F521C1-04A8-45D3-9C26-AF01B3A5FFCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{A6D1979C-1509-4C46-98AF-D9F73C578E15}"/>
   </bookViews>
@@ -1031,8 +1031,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08D947E0-304F-4500-988F-A4F88753FC79}">
   <dimension ref="A1:AGG22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BJ1" workbookViewId="0">
-      <selection activeCell="GC9" sqref="GC9"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>